<commit_message>
not us17/16 but 15/16
</commit_message>
<xml_diff>
--- a/TeamAustinMichaelOscarTarikReport_Sprint_3.xlsx
+++ b/TeamAustinMichaelOscarTarikReport_Sprint_3.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr date1904="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C954C718-43C4-4187-A225-E5C151D25600}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B9B12DC5-DDD4-40FE-9CEE-C87F23B82121}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="6225" tabRatio="832" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13140" windowHeight="6225" tabRatio="832" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="179017" concurrentCalc="0"/>
-  <oleSize ref="A1:J21"/>
+  <oleSize ref="B13:E21"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -3690,7 +3690,7 @@
     <col min="3" max="3" width="25.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>41710</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3786,7 +3786,7 @@
         <v>41712</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>41712</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>41713</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>41713</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>41713</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>41716</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>41717</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
@@ -3987,7 +3987,7 @@
       <c r="I10" s="17"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C11" s="5" t="s">
         <v>31</v>
       </c>
@@ -3996,14 +3996,14 @@
       <c r="F11" s="17"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C13" s="5" t="s">
         <v>32</v>
       </c>
@@ -4012,7 +4012,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C14" s="19" t="s">
         <v>203</v>
       </c>
@@ -4022,34 +4022,34 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="3:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C17" s="5" t="s">
         <v>33</v>
       </c>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="3:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C18" s="19" t="s">
         <v>205</v>
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="3:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="3:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="3:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="3:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="3:10" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="3:10" ht="12.6" x14ac:dyDescent="0.2">
@@ -4149,7 +4149,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4294,7 +4294,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -4323,13 +4323,13 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:9" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
@@ -4346,7 +4346,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+    <sheetView zoomScale="98" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -4420,8 +4420,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>